<commit_message>
feat: Send Swagger docs
</commit_message>
<xml_diff>
--- a/CV de compétences.xlsx
+++ b/CV de compétences.xlsx
@@ -5,44 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shagr\Documents\Simplon\Niort CDA - Maif 2024\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shagr\Documents\Simplon\Niort CDA - Maif 2024\simplon-2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{003F7D5B-A736-41AB-B19F-7545A49FF6D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A485347-A8B9-449C-BDBE-9199392C7B5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="19543" windowHeight="12377" xr2:uid="{B0B99F8E-B04E-4401-A49C-3631BDFA6790}"/>
+    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{B0B99F8E-B04E-4401-A49C-3631BDFA6790}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Feuil1!$A$19</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Feuil1!$A$21:$B$21</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Feuil1!$C$21</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Feuil1!$C$2:$C$21</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">Feuil1!$C$30</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Feuil1!$A$19</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">Feuil1!$A$21:$B$21</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">Feuil1!$A$30</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">Feuil1!$A$30:$C$30</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">Feuil1!$B$1</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">Feuil1!$B$2:$B$21</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">Feuil1!$B$2:$C$21</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Feuil1!$A$30</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">Feuil1!$B$30</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">Feuil1!$C$1</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">Feuil1!$C$1:$C$20</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">Feuil1!$C$21</definedName>
-    <definedName name="_xlchart.v1.24" hidden="1">Feuil1!$C$2:$C$21</definedName>
-    <definedName name="_xlchart.v1.25" hidden="1">Feuil1!$C$30</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Feuil1!$A$30:$C$30</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Feuil1!$B$1</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Feuil1!$B$2:$B$21</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Feuil1!$B$2:$C$21</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Feuil1!$B$30</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Feuil1!$C$1</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Feuil1!$C$1:$C$20</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1633,7 +1605,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>

</xml_diff>